<commit_message>
Corrigido importação por excel
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/ModeloMonitorador.xlsx
+++ b/src/main/resources/excel/ModeloMonitorador.xlsx
@@ -122,16 +122,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="17.53515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="14.07421875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="19.87890625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="13.796875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="7.515625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="3.80859375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.47265625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="20.30078125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="10.09375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="18.140625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="19.55078125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="15.6953125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="22.16796875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.3828125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="8.37890625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.24609375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.79296875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="22.63671875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="11.25390625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -167,34 +167,34 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>